<commit_message>
minor changes - file formatting etc
</commit_message>
<xml_diff>
--- a/test_results/results_export.xlsx
+++ b/test_results/results_export.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,11 +446,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Serial Test</t>
+          <t>Poker Test</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.756</v>
+        <v>0.855</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -458,17 +458,35 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3906</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Two Bit Test</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.385</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Serial Test</t>
+          <t>Gap Test</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.956</v>
+        <v>0.625</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -476,17 +494,35 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3933</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Turning Point Test</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.227</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Serial Test</t>
+          <t>Autocorrelation Test</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.377</v>
+        <v>0.575</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -494,17 +530,35 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4181</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Hamming Weight Test</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.9379999999999999</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Serial Test</t>
+          <t>Monobit</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.385</v>
+        <v>0.589</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -512,17 +566,35 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>4044</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Frequency Within Block</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.8070000000000001</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Serial Test</t>
+          <t>Runs</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.256</v>
+        <v>0.253</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -530,17 +602,35 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3919</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Longest Run Ones In A Block</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.585</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Serial Test</t>
+          <t>Discrete Fourier Transform</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.64</v>
+        <v>0.783</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -548,7 +638,25 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3955</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Non Overlapping Template Matching</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="15">
@@ -558,7 +666,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.174</v>
+        <v>0.915</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -566,17 +674,35 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>4081</v>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Approximate Entropy</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.741</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>531</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Serial Test</t>
+          <t>Cumulative Sums</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.603</v>
+        <v>0.739</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -584,17 +710,35 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>4022</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Random Excursion</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Serial Test</t>
+          <t>Random Excursion Variant</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.785</v>
+        <v>0.432</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -602,25 +746,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>3957</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Serial Test</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0.119</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>3981</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>